<commit_message>
v1 for added imu raw data
</commit_message>
<xml_diff>
--- a/postflight/main_flight/aurora_flight_data.xlsx
+++ b/postflight/main_flight/aurora_flight_data.xlsx
@@ -10,6 +10,7 @@
     <sheet name="proc_cmd" sheetId="1" state="visible" r:id="rId1"/>
     <sheet name="mcb_encoder" sheetId="2" state="visible" r:id="rId2"/>
     <sheet name="state_est_data" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="altimu_meas" sheetId="4" state="visible" r:id="rId4"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -54704,4 +54705,1840 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:C121"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>time_ms</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>data_id</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>value</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>24712</v>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>SENSOR_IMU_Z</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>{'3996', '7686'}</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>24712</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>SENSOR_MAG_X</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>{'64871'}</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>24712</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>SENSOR_MAG_Y</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>{'906'}</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>24712</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>SENSOR_MAG_Z</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>{'965'}</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>24712</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>SENSOR_BARO</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>{'3226', '2213225'}</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>25029</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>SENSOR_IMU_X</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>{'63812', '69'}</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>25029</v>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>SENSOR_IMU_Y</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>{'654', '582'}</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>25029</v>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>SENSOR_IMU_Z</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>{'4564', '7823'}</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>25029</v>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>SENSOR_MAG_X</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>{'64335'}</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>25029</v>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>SENSOR_MAG_Y</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>{'502'}</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>25029</v>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>SENSOR_MAG_Z</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>{'943'}</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>25029</v>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>SENSOR_BARO</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>{'2175746', '3211'}</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="n">
+        <v>25029</v>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>SENSOR_BARO</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>{'2175746', '3211'}</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="n">
+        <v>39917</v>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>SENSOR_IMU_X</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>{'27', '65499'}</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="n">
+        <v>39917</v>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>SENSOR_IMU_Y</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>{'65493', '21'}</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="n">
+        <v>39917</v>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>SENSOR_IMU_Z</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>{'64884', '806'}</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="n">
+        <v>40237</v>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>SENSOR_IMU_X</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>{'65500', '65535'}</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="n">
+        <v>40237</v>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>SENSOR_IMU_Y</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>{'44', '65423'}</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="n">
+        <v>40237</v>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>SENSOR_IMU_Z</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>{'65018', '750'}</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="n">
+        <v>40237</v>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>SENSOR_MAG_X</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>{'63952'}</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="n">
+        <v>40237</v>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>SENSOR_MAG_Y</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>{'924'}</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="n">
+        <v>40237</v>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>SENSOR_MAG_Z</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>{'896'}</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="n">
+        <v>40237</v>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>SENSOR_BARO</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>{'1115428', '3258'}</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="n">
+        <v>55125</v>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>SENSOR_BARO</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>{'3245', '819957'}</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="n">
+        <v>55229</v>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>SENSOR_IMU_X</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>{'65510', '65522'}</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="n">
+        <v>55229</v>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>SENSOR_IMU_Y</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>{'65532', '65477'}</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="n">
+        <v>55229</v>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>SENSOR_IMU_Z</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>{'1089', '164'}</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="n">
+        <v>55440</v>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>SENSOR_IMU_X</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>{'65519', '65477'}</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="n">
+        <v>55440</v>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>SENSOR_IMU_Y</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>{'65491', '65520'}</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="n">
+        <v>55440</v>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>SENSOR_IMU_Z</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>{'159', '1155'}</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="n">
+        <v>55440</v>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>SENSOR_MAG_X</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>{'65174'}</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="n">
+        <v>55440</v>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>SENSOR_MAG_Y</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>{'1232'}</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="n">
+        <v>55440</v>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>SENSOR_MAG_Z</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>{'700'}</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="n">
+        <v>55440</v>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>SENSOR_BARO</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>{'3245', '818682'}</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="n">
+        <v>55546</v>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>SENSOR_IMU_X</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>{'65506', '65516'}</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="n">
+        <v>70327</v>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>SENSOR_IMU_X</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>{'22', '15'}</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="n">
+        <v>70327</v>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>SENSOR_IMU_Y</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>{'65475', '100'}</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="n">
+        <v>70327</v>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>SENSOR_IMU_Z</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>{'313', '649'}</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="n">
+        <v>70327</v>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>SENSOR_MAG_X</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>{'64857'}</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="n">
+        <v>70327</v>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>SENSOR_MAG_Y</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>{'1531'}</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="n">
+        <v>70327</v>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>SENSOR_MAG_Z</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>{'65194'}</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="n">
+        <v>70327</v>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>SENSOR_BARO</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>{'799316', '3141'}</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="n">
+        <v>85426</v>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>SENSOR_IMU_Y</t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>{'65137', '6'}</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="n">
+        <v>85426</v>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>SENSOR_IMU_Z</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>{'1094', '905'}</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="n">
+        <v>85426</v>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>SENSOR_MAG_X</t>
+        </is>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>{'64876'}</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="n">
+        <v>85426</v>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>SENSOR_MAG_Y</t>
+        </is>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>{'824'}</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="n">
+        <v>85426</v>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>SENSOR_MAG_Z</t>
+        </is>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>{'64868'}</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="n">
+        <v>85426</v>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>SENSOR_BARO</t>
+        </is>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>{'1019289', '2806'}</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="n">
+        <v>85532</v>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>SENSOR_IMU_X</t>
+        </is>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>{'65484', '65514'}</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="n">
+        <v>85532</v>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>SENSOR_IMU_Y</t>
+        </is>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>{'24', '2'}</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="n">
+        <v>85532</v>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>SENSOR_IMU_Z</t>
+        </is>
+      </c>
+      <c r="C52" t="inlineStr">
+        <is>
+          <t>{'1053', '940'}</t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="n">
+        <v>85532</v>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>SENSOR_MAG_X</t>
+        </is>
+      </c>
+      <c r="C53" t="inlineStr">
+        <is>
+          <t>{'64862'}</t>
+        </is>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="n">
+        <v>85532</v>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>SENSOR_MAG_Y</t>
+        </is>
+      </c>
+      <c r="C54" t="inlineStr">
+        <is>
+          <t>{'771'}</t>
+        </is>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="n">
+        <v>85532</v>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>SENSOR_MAG_Z</t>
+        </is>
+      </c>
+      <c r="C55" t="inlineStr">
+        <is>
+          <t>{'64853'}</t>
+        </is>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="n">
+        <v>85532</v>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>SENSOR_BARO</t>
+        </is>
+      </c>
+      <c r="C56" t="inlineStr">
+        <is>
+          <t>{'1016676', '2804'}</t>
+        </is>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="n">
+        <v>85743</v>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>SENSOR_IMU_X</t>
+        </is>
+      </c>
+      <c r="C57" t="inlineStr">
+        <is>
+          <t>{'65508', '65447'}</t>
+        </is>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="n">
+        <v>85743</v>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>SENSOR_IMU_Y</t>
+        </is>
+      </c>
+      <c r="C58" t="inlineStr">
+        <is>
+          <t>{'65526', '65272'}</t>
+        </is>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="n">
+        <v>85743</v>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>SENSOR_IMU_Z</t>
+        </is>
+      </c>
+      <c r="C59" t="inlineStr">
+        <is>
+          <t>{'919', '905'}</t>
+        </is>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="n">
+        <v>85743</v>
+      </c>
+      <c r="B60" t="inlineStr">
+        <is>
+          <t>SENSOR_MAG_X</t>
+        </is>
+      </c>
+      <c r="C60" t="inlineStr">
+        <is>
+          <t>{'64823'}</t>
+        </is>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="n">
+        <v>85743</v>
+      </c>
+      <c r="B61" t="inlineStr">
+        <is>
+          <t>SENSOR_MAG_Y</t>
+        </is>
+      </c>
+      <c r="C61" t="inlineStr">
+        <is>
+          <t>{'688'}</t>
+        </is>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="n">
+        <v>85743</v>
+      </c>
+      <c r="B62" t="inlineStr">
+        <is>
+          <t>SENSOR_MAG_Z</t>
+        </is>
+      </c>
+      <c r="C62" t="inlineStr">
+        <is>
+          <t>{'64854'}</t>
+        </is>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="n">
+        <v>85743</v>
+      </c>
+      <c r="B63" t="inlineStr">
+        <is>
+          <t>SENSOR_BARO</t>
+        </is>
+      </c>
+      <c r="C63" t="inlineStr">
+        <is>
+          <t>{'2803', '1027103'}</t>
+        </is>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="n">
+        <v>100738</v>
+      </c>
+      <c r="B64" t="inlineStr">
+        <is>
+          <t>SENSOR_IMU_Y</t>
+        </is>
+      </c>
+      <c r="C64" t="inlineStr">
+        <is>
+          <t>{'17', '65202'}</t>
+        </is>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="n">
+        <v>100738</v>
+      </c>
+      <c r="B65" t="inlineStr">
+        <is>
+          <t>SENSOR_IMU_Z</t>
+        </is>
+      </c>
+      <c r="C65" t="inlineStr">
+        <is>
+          <t>{'6', '1792'}</t>
+        </is>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="n">
+        <v>100738</v>
+      </c>
+      <c r="B66" t="inlineStr">
+        <is>
+          <t>SENSOR_MAG_X</t>
+        </is>
+      </c>
+      <c r="C66" t="inlineStr">
+        <is>
+          <t>{'64201'}</t>
+        </is>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="n">
+        <v>100738</v>
+      </c>
+      <c r="B67" t="inlineStr">
+        <is>
+          <t>SENSOR_MAG_Y</t>
+        </is>
+      </c>
+      <c r="C67" t="inlineStr">
+        <is>
+          <t>{'1013'}</t>
+        </is>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="n">
+        <v>100738</v>
+      </c>
+      <c r="B68" t="inlineStr">
+        <is>
+          <t>SENSOR_MAG_Z</t>
+        </is>
+      </c>
+      <c r="C68" t="inlineStr">
+        <is>
+          <t>{'64799'}</t>
+        </is>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="n">
+        <v>100738</v>
+      </c>
+      <c r="B69" t="inlineStr">
+        <is>
+          <t>SENSOR_BARO</t>
+        </is>
+      </c>
+      <c r="C69" t="inlineStr">
+        <is>
+          <t>{'2313', '1487106'}</t>
+        </is>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="n">
+        <v>100950</v>
+      </c>
+      <c r="B70" t="inlineStr">
+        <is>
+          <t>SENSOR_IMU_X</t>
+        </is>
+      </c>
+      <c r="C70" t="inlineStr">
+        <is>
+          <t>{'30', '79'}</t>
+        </is>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="n">
+        <v>100950</v>
+      </c>
+      <c r="B71" t="inlineStr">
+        <is>
+          <t>SENSOR_IMU_Y</t>
+        </is>
+      </c>
+      <c r="C71" t="inlineStr">
+        <is>
+          <t>{'9', '65403'}</t>
+        </is>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="n">
+        <v>100950</v>
+      </c>
+      <c r="B72" t="inlineStr">
+        <is>
+          <t>SENSOR_IMU_Z</t>
+        </is>
+      </c>
+      <c r="C72" t="inlineStr">
+        <is>
+          <t>{'1892', '116'}</t>
+        </is>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="n">
+        <v>100950</v>
+      </c>
+      <c r="B73" t="inlineStr">
+        <is>
+          <t>SENSOR_MAG_X</t>
+        </is>
+      </c>
+      <c r="C73" t="inlineStr">
+        <is>
+          <t>{'64220'}</t>
+        </is>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="n">
+        <v>100950</v>
+      </c>
+      <c r="B74" t="inlineStr">
+        <is>
+          <t>SENSOR_MAG_Y</t>
+        </is>
+      </c>
+      <c r="C74" t="inlineStr">
+        <is>
+          <t>{'1003'}</t>
+        </is>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="n">
+        <v>100950</v>
+      </c>
+      <c r="B75" t="inlineStr">
+        <is>
+          <t>SENSOR_MAG_Y</t>
+        </is>
+      </c>
+      <c r="C75" t="inlineStr">
+        <is>
+          <t>{'1003'}</t>
+        </is>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="n">
+        <v>100950</v>
+      </c>
+      <c r="B76" t="inlineStr">
+        <is>
+          <t>SENSOR_MAG_Z</t>
+        </is>
+      </c>
+      <c r="C76" t="inlineStr">
+        <is>
+          <t>{'64664'}</t>
+        </is>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="n">
+        <v>100950</v>
+      </c>
+      <c r="B77" t="inlineStr">
+        <is>
+          <t>SENSOR_BARO</t>
+        </is>
+      </c>
+      <c r="C77" t="inlineStr">
+        <is>
+          <t>{'1494342', '2308'}</t>
+        </is>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="n">
+        <v>115945</v>
+      </c>
+      <c r="B78" t="inlineStr">
+        <is>
+          <t>SENSOR_IMU_Z</t>
+        </is>
+      </c>
+      <c r="C78" t="inlineStr">
+        <is>
+          <t>{'64991', '2021'}</t>
+        </is>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="n">
+        <v>115945</v>
+      </c>
+      <c r="B79" t="inlineStr">
+        <is>
+          <t>SENSOR_MAG_X</t>
+        </is>
+      </c>
+      <c r="C79" t="inlineStr">
+        <is>
+          <t>{'64393'}</t>
+        </is>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="n">
+        <v>115945</v>
+      </c>
+      <c r="B80" t="inlineStr">
+        <is>
+          <t>SENSOR_MAG_Y</t>
+        </is>
+      </c>
+      <c r="C80" t="inlineStr">
+        <is>
+          <t>{'1087'}</t>
+        </is>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="n">
+        <v>115945</v>
+      </c>
+      <c r="B81" t="inlineStr">
+        <is>
+          <t>SENSOR_MAG_Z</t>
+        </is>
+      </c>
+      <c r="C81" t="inlineStr">
+        <is>
+          <t>{'64771'}</t>
+        </is>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="n">
+        <v>115945</v>
+      </c>
+      <c r="B82" t="inlineStr">
+        <is>
+          <t>SENSOR_BARO</t>
+        </is>
+      </c>
+      <c r="C82" t="inlineStr">
+        <is>
+          <t>{'2105', '2161418'}</t>
+        </is>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="n">
+        <v>116260</v>
+      </c>
+      <c r="B83" t="inlineStr">
+        <is>
+          <t>SENSOR_IMU_X</t>
+        </is>
+      </c>
+      <c r="C83" t="inlineStr">
+        <is>
+          <t>{'64950', '61'}</t>
+        </is>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="n">
+        <v>116260</v>
+      </c>
+      <c r="B84" t="inlineStr">
+        <is>
+          <t>SENSOR_IMU_Y</t>
+        </is>
+      </c>
+      <c r="C84" t="inlineStr">
+        <is>
+          <t>{'65421', '65475'}</t>
+        </is>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="n">
+        <v>116260</v>
+      </c>
+      <c r="B85" t="inlineStr">
+        <is>
+          <t>SENSOR_IMU_Z</t>
+        </is>
+      </c>
+      <c r="C85" t="inlineStr">
+        <is>
+          <t>{'2146', '64988'}</t>
+        </is>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="n">
+        <v>116260</v>
+      </c>
+      <c r="B86" t="inlineStr">
+        <is>
+          <t>SENSOR_MAG_X</t>
+        </is>
+      </c>
+      <c r="C86" t="inlineStr">
+        <is>
+          <t>{'64367'}</t>
+        </is>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="n">
+        <v>116260</v>
+      </c>
+      <c r="B87" t="inlineStr">
+        <is>
+          <t>SENSOR_MAG_Y</t>
+        </is>
+      </c>
+      <c r="C87" t="inlineStr">
+        <is>
+          <t>{'1084'}</t>
+        </is>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="n">
+        <v>116260</v>
+      </c>
+      <c r="B88" t="inlineStr">
+        <is>
+          <t>SENSOR_MAG_Z</t>
+        </is>
+      </c>
+      <c r="C88" t="inlineStr">
+        <is>
+          <t>{'64759'}</t>
+        </is>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="n">
+        <v>116260</v>
+      </c>
+      <c r="B89" t="inlineStr">
+        <is>
+          <t>SENSOR_BARO</t>
+        </is>
+      </c>
+      <c r="C89" t="inlineStr">
+        <is>
+          <t>{'2106', '2158255'}</t>
+        </is>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="n">
+        <v>116366</v>
+      </c>
+      <c r="B90" t="inlineStr">
+        <is>
+          <t>SENSOR_IMU_X</t>
+        </is>
+      </c>
+      <c r="C90" t="inlineStr">
+        <is>
+          <t>{'64644', '24'}</t>
+        </is>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="n">
+        <v>116366</v>
+      </c>
+      <c r="B91" t="inlineStr">
+        <is>
+          <t>SENSOR_IMU_Y</t>
+        </is>
+      </c>
+      <c r="C91" t="inlineStr">
+        <is>
+          <t>{'65531', '31'}</t>
+        </is>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="n">
+        <v>116366</v>
+      </c>
+      <c r="B92" t="inlineStr">
+        <is>
+          <t>SENSOR_IMU_Z</t>
+        </is>
+      </c>
+      <c r="C92" t="inlineStr">
+        <is>
+          <t>{'64817', '2256'}</t>
+        </is>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="n">
+        <v>116366</v>
+      </c>
+      <c r="B93" t="inlineStr">
+        <is>
+          <t>SENSOR_MAG_X</t>
+        </is>
+      </c>
+      <c r="C93" t="inlineStr">
+        <is>
+          <t>{'64359'}</t>
+        </is>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="n">
+        <v>116366</v>
+      </c>
+      <c r="B94" t="inlineStr">
+        <is>
+          <t>SENSOR_MAG_Y</t>
+        </is>
+      </c>
+      <c r="C94" t="inlineStr">
+        <is>
+          <t>{'1070'}</t>
+        </is>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="n">
+        <v>131253</v>
+      </c>
+      <c r="B95" t="inlineStr">
+        <is>
+          <t>SENSOR_IMU_X</t>
+        </is>
+      </c>
+      <c r="C95" t="inlineStr">
+        <is>
+          <t>{'64640', '57'}</t>
+        </is>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" t="n">
+        <v>131253</v>
+      </c>
+      <c r="B96" t="inlineStr">
+        <is>
+          <t>SENSOR_IMU_Y</t>
+        </is>
+      </c>
+      <c r="C96" t="inlineStr">
+        <is>
+          <t>{'65244', '65535'}</t>
+        </is>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" t="n">
+        <v>131253</v>
+      </c>
+      <c r="B97" t="inlineStr">
+        <is>
+          <t>SENSOR_IMU_Z</t>
+        </is>
+      </c>
+      <c r="C97" t="inlineStr">
+        <is>
+          <t>{'63759', '2266'}</t>
+        </is>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" t="n">
+        <v>131253</v>
+      </c>
+      <c r="B98" t="inlineStr">
+        <is>
+          <t>SENSOR_MAG_X</t>
+        </is>
+      </c>
+      <c r="C98" t="inlineStr">
+        <is>
+          <t>{'64641'}</t>
+        </is>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" t="n">
+        <v>131253</v>
+      </c>
+      <c r="B99" t="inlineStr">
+        <is>
+          <t>SENSOR_MAG_Y</t>
+        </is>
+      </c>
+      <c r="C99" t="inlineStr">
+        <is>
+          <t>{'1118'}</t>
+        </is>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" t="n">
+        <v>131253</v>
+      </c>
+      <c r="B100" t="inlineStr">
+        <is>
+          <t>SENSOR_MAG_Z</t>
+        </is>
+      </c>
+      <c r="C100" t="inlineStr">
+        <is>
+          <t>{'64793'}</t>
+        </is>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" t="n">
+        <v>131253</v>
+      </c>
+      <c r="B101" t="inlineStr">
+        <is>
+          <t>SENSOR_BARO</t>
+        </is>
+      </c>
+      <c r="C101" t="inlineStr">
+        <is>
+          <t>{'2088', '2977769'}</t>
+        </is>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" t="n">
+        <v>131569</v>
+      </c>
+      <c r="B102" t="inlineStr">
+        <is>
+          <t>SENSOR_IMU_X</t>
+        </is>
+      </c>
+      <c r="C102" t="inlineStr">
+        <is>
+          <t>{'65063', '52'}</t>
+        </is>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" t="n">
+        <v>131569</v>
+      </c>
+      <c r="B103" t="inlineStr">
+        <is>
+          <t>SENSOR_IMU_Y</t>
+        </is>
+      </c>
+      <c r="C103" t="inlineStr">
+        <is>
+          <t>{'104', '96'}</t>
+        </is>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" t="n">
+        <v>131569</v>
+      </c>
+      <c r="B104" t="inlineStr">
+        <is>
+          <t>SENSOR_IMU_Z</t>
+        </is>
+      </c>
+      <c r="C104" t="inlineStr">
+        <is>
+          <t>{'2461', '63520'}</t>
+        </is>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" t="n">
+        <v>131569</v>
+      </c>
+      <c r="B105" t="inlineStr">
+        <is>
+          <t>SENSOR_MAG_X</t>
+        </is>
+      </c>
+      <c r="C105" t="inlineStr">
+        <is>
+          <t>{'64425'}</t>
+        </is>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" t="n">
+        <v>131569</v>
+      </c>
+      <c r="B106" t="inlineStr">
+        <is>
+          <t>SENSOR_MAG_Y</t>
+        </is>
+      </c>
+      <c r="C106" t="inlineStr">
+        <is>
+          <t>{'1136'}</t>
+        </is>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" t="n">
+        <v>131569</v>
+      </c>
+      <c r="B107" t="inlineStr">
+        <is>
+          <t>SENSOR_MAG_Z</t>
+        </is>
+      </c>
+      <c r="C107" t="inlineStr">
+        <is>
+          <t>{'64790'}</t>
+        </is>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" t="n">
+        <v>146457</v>
+      </c>
+      <c r="B108" t="inlineStr">
+        <is>
+          <t>SENSOR_IMU_X</t>
+        </is>
+      </c>
+      <c r="C108" t="inlineStr">
+        <is>
+          <t>{'65062', '65469'}</t>
+        </is>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109" t="n">
+        <v>146457</v>
+      </c>
+      <c r="B109" t="inlineStr">
+        <is>
+          <t>SENSOR_IMU_Y</t>
+        </is>
+      </c>
+      <c r="C109" t="inlineStr">
+        <is>
+          <t>{'118', '65304'}</t>
+        </is>
+      </c>
+    </row>
+    <row r="110">
+      <c r="A110" t="n">
+        <v>146457</v>
+      </c>
+      <c r="B110" t="inlineStr">
+        <is>
+          <t>SENSOR_IMU_Z</t>
+        </is>
+      </c>
+      <c r="C110" t="inlineStr">
+        <is>
+          <t>{'64204', '2241'}</t>
+        </is>
+      </c>
+    </row>
+    <row r="111">
+      <c r="A111" t="n">
+        <v>146457</v>
+      </c>
+      <c r="B111" t="inlineStr">
+        <is>
+          <t>SENSOR_MAG_X</t>
+        </is>
+      </c>
+      <c r="C111" t="inlineStr">
+        <is>
+          <t>{'64209'}</t>
+        </is>
+      </c>
+    </row>
+    <row r="112">
+      <c r="A112" t="n">
+        <v>146457</v>
+      </c>
+      <c r="B112" t="inlineStr">
+        <is>
+          <t>SENSOR_MAG_Y</t>
+        </is>
+      </c>
+      <c r="C112" t="inlineStr">
+        <is>
+          <t>{'918'}</t>
+        </is>
+      </c>
+    </row>
+    <row r="113">
+      <c r="A113" t="n">
+        <v>146457</v>
+      </c>
+      <c r="B113" t="inlineStr">
+        <is>
+          <t>SENSOR_MAG_Z</t>
+        </is>
+      </c>
+      <c r="C113" t="inlineStr">
+        <is>
+          <t>{'64761'}</t>
+        </is>
+      </c>
+    </row>
+    <row r="114">
+      <c r="A114" t="n">
+        <v>146457</v>
+      </c>
+      <c r="B114" t="inlineStr">
+        <is>
+          <t>SENSOR_BARO</t>
+        </is>
+      </c>
+      <c r="C114" t="inlineStr">
+        <is>
+          <t>{'3912278', '2174'}</t>
+        </is>
+      </c>
+    </row>
+    <row r="115">
+      <c r="A115" t="n">
+        <v>146563</v>
+      </c>
+      <c r="B115" t="inlineStr">
+        <is>
+          <t>SENSOR_IMU_X</t>
+        </is>
+      </c>
+      <c r="C115" t="inlineStr">
+        <is>
+          <t>{'446', '65401'}</t>
+        </is>
+      </c>
+    </row>
+    <row r="116">
+      <c r="A116" t="n">
+        <v>146774</v>
+      </c>
+      <c r="B116" t="inlineStr">
+        <is>
+          <t>SENSOR_IMU_X</t>
+        </is>
+      </c>
+      <c r="C116" t="inlineStr">
+        <is>
+          <t>{'54', '45'}</t>
+        </is>
+      </c>
+    </row>
+    <row r="117">
+      <c r="A117" t="n">
+        <v>146774</v>
+      </c>
+      <c r="B117" t="inlineStr">
+        <is>
+          <t>SENSOR_IMU_Y</t>
+        </is>
+      </c>
+      <c r="C117" t="inlineStr">
+        <is>
+          <t>{'48', '64657'}</t>
+        </is>
+      </c>
+    </row>
+    <row r="118">
+      <c r="A118" t="n">
+        <v>146774</v>
+      </c>
+      <c r="B118" t="inlineStr">
+        <is>
+          <t>SENSOR_IMU_Z</t>
+        </is>
+      </c>
+      <c r="C118" t="inlineStr">
+        <is>
+          <t>{'2550', '64365'}</t>
+        </is>
+      </c>
+    </row>
+    <row r="119">
+      <c r="A119" t="n">
+        <v>146774</v>
+      </c>
+      <c r="B119" t="inlineStr">
+        <is>
+          <t>SENSOR_MAG_X</t>
+        </is>
+      </c>
+      <c r="C119" t="inlineStr">
+        <is>
+          <t>{'64196'}</t>
+        </is>
+      </c>
+    </row>
+    <row r="120">
+      <c r="A120" t="n">
+        <v>146774</v>
+      </c>
+      <c r="B120" t="inlineStr">
+        <is>
+          <t>SENSOR_MAG_Y</t>
+        </is>
+      </c>
+      <c r="C120" t="inlineStr">
+        <is>
+          <t>{'789'}</t>
+        </is>
+      </c>
+    </row>
+    <row r="121">
+      <c r="A121" t="n">
+        <v>146774</v>
+      </c>
+      <c r="B121" t="inlineStr">
+        <is>
+          <t>SENSOR_MAG_Z</t>
+        </is>
+      </c>
+      <c r="C121" t="inlineStr">
+        <is>
+          <t>{'64752'}</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
final version thats so much cleaner
</commit_message>
<xml_diff>
--- a/postflight/main_flight/aurora_flight_data.xlsx
+++ b/postflight/main_flight/aurora_flight_data.xlsx
@@ -40,7 +40,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -54,15 +54,37 @@
       <top style="thin"/>
       <bottom style="thin"/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin"/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -54612,7 +54634,6 @@
           <t>STATE_ID_RATE_WX</t>
         </is>
       </c>
-      <c r="C162" t="inlineStr"/>
     </row>
     <row r="163">
       <c r="A163" t="n">
@@ -54623,7 +54644,6 @@
           <t>STATE_ID_RATE_WY</t>
         </is>
       </c>
-      <c r="C163" t="inlineStr"/>
     </row>
     <row r="164">
       <c r="A164" t="n">
@@ -54634,7 +54654,6 @@
           <t>STATE_ID_RATE_WZ</t>
         </is>
       </c>
-      <c r="C164" t="inlineStr"/>
     </row>
     <row r="165">
       <c r="A165" t="n">
@@ -54645,7 +54664,6 @@
           <t>STATE_ID_VEL_VX</t>
         </is>
       </c>
-      <c r="C165" t="inlineStr"/>
     </row>
     <row r="166">
       <c r="A166" t="n">
@@ -54656,7 +54674,6 @@
           <t>STATE_ID_VEL_VY</t>
         </is>
       </c>
-      <c r="C166" t="inlineStr"/>
     </row>
     <row r="167">
       <c r="A167" t="n">
@@ -54667,7 +54684,6 @@
           <t>STATE_ID_VEL_VZ</t>
         </is>
       </c>
-      <c r="C167" t="inlineStr"/>
     </row>
     <row r="168">
       <c r="A168" t="n">
@@ -54678,7 +54694,6 @@
           <t>STATE_ID_ALT</t>
         </is>
       </c>
-      <c r="C168" t="inlineStr"/>
     </row>
     <row r="169">
       <c r="A169" t="n">
@@ -54689,7 +54704,6 @@
           <t>STATE_ID_COEFF_CL</t>
         </is>
       </c>
-      <c r="C169" t="inlineStr"/>
     </row>
     <row r="170">
       <c r="A170" t="n">
@@ -54700,7 +54714,6 @@
           <t>STATE_ID_CANARD_ANGLE</t>
         </is>
       </c>
-      <c r="C170" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -54713,7 +54726,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C121"/>
+  <dimension ref="A1:L24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -54722,1823 +54735,784 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="inlineStr">
+      <c r="A1" s="1" t="inlineStr"/>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>SENSOR_BARO</t>
+        </is>
+      </c>
+      <c r="C1" s="2" t="n"/>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>SENSOR_IMU_X</t>
+        </is>
+      </c>
+      <c r="E1" s="2" t="n"/>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>SENSOR_IMU_Y</t>
+        </is>
+      </c>
+      <c r="G1" s="2" t="n"/>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>SENSOR_IMU_Z</t>
+        </is>
+      </c>
+      <c r="I1" s="2" t="n"/>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>SENSOR_MAG_X</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>SENSOR_MAG_Y</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>SENSOR_MAG_Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="inlineStr">
         <is>
           <t>time_ms</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
+      <c r="B2" s="1" t="inlineStr">
         <is>
-          <t>data_id</t>
+          <t>pressure:</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="C2" s="1" t="inlineStr">
         <is>
-          <t>value</t>
+          <t>temp:</t>
         </is>
       </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="n">
+      <c r="D2" s="1" t="inlineStr">
+        <is>
+          <t>angular_velocity:</t>
+        </is>
+      </c>
+      <c r="E2" s="1" t="inlineStr">
+        <is>
+          <t>linear_accel:</t>
+        </is>
+      </c>
+      <c r="F2" s="1" t="inlineStr">
+        <is>
+          <t>angular_velocity:</t>
+        </is>
+      </c>
+      <c r="G2" s="1" t="inlineStr">
+        <is>
+          <t>linear_accel:</t>
+        </is>
+      </c>
+      <c r="H2" s="1" t="inlineStr">
+        <is>
+          <t>angular_velocity:</t>
+        </is>
+      </c>
+      <c r="I2" s="1" t="inlineStr">
+        <is>
+          <t>linear_accel:</t>
+        </is>
+      </c>
+      <c r="J2" s="1" t="inlineStr">
+        <is>
+          <t>mag:</t>
+        </is>
+      </c>
+      <c r="K2" s="1" t="inlineStr">
+        <is>
+          <t>mag:</t>
+        </is>
+      </c>
+      <c r="L2" s="1" t="inlineStr">
+        <is>
+          <t>mag:</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="n">
         <v>24712</v>
       </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>SENSOR_IMU_Z</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>{'3996', '7686'}</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="n">
-        <v>24712</v>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>SENSOR_MAG_X</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>{'64871'}</t>
-        </is>
+      <c r="B3" t="n">
+        <v>2213225</v>
+      </c>
+      <c r="C3" t="n">
+        <v>3226</v>
+      </c>
+      <c r="H3" t="n">
+        <v>3996</v>
+      </c>
+      <c r="I3" t="n">
+        <v>7686</v>
+      </c>
+      <c r="J3" t="n">
+        <v>64871</v>
+      </c>
+      <c r="K3" t="n">
+        <v>906</v>
+      </c>
+      <c r="L3" t="n">
+        <v>965</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="n">
-        <v>24712</v>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>SENSOR_MAG_Y</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>{'906'}</t>
-        </is>
+      <c r="A4" s="1" t="n">
+        <v>25029</v>
+      </c>
+      <c r="B4" t="n">
+        <v>2175746</v>
+      </c>
+      <c r="C4" t="n">
+        <v>3211</v>
+      </c>
+      <c r="D4" t="n">
+        <v>69</v>
+      </c>
+      <c r="E4" t="n">
+        <v>63812</v>
+      </c>
+      <c r="F4" t="n">
+        <v>582</v>
+      </c>
+      <c r="G4" t="n">
+        <v>654</v>
+      </c>
+      <c r="H4" t="n">
+        <v>4564</v>
+      </c>
+      <c r="I4" t="n">
+        <v>7823</v>
+      </c>
+      <c r="J4" t="n">
+        <v>64335</v>
+      </c>
+      <c r="K4" t="n">
+        <v>502</v>
+      </c>
+      <c r="L4" t="n">
+        <v>943</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" t="n">
-        <v>24712</v>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>SENSOR_MAG_Z</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>{'965'}</t>
-        </is>
+      <c r="A5" s="1" t="n">
+        <v>39917</v>
+      </c>
+      <c r="D5" t="n">
+        <v>27</v>
+      </c>
+      <c r="E5" t="n">
+        <v>65499</v>
+      </c>
+      <c r="F5" t="n">
+        <v>65493</v>
+      </c>
+      <c r="G5" t="n">
+        <v>21</v>
+      </c>
+      <c r="H5" t="n">
+        <v>64884</v>
+      </c>
+      <c r="I5" t="n">
+        <v>806</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" t="n">
-        <v>24712</v>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>SENSOR_BARO</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>{'3226', '2213225'}</t>
-        </is>
+      <c r="A6" s="1" t="n">
+        <v>40237</v>
+      </c>
+      <c r="B6" t="n">
+        <v>1115428</v>
+      </c>
+      <c r="C6" t="n">
+        <v>3258</v>
+      </c>
+      <c r="D6" t="n">
+        <v>65535</v>
+      </c>
+      <c r="E6" t="n">
+        <v>65500</v>
+      </c>
+      <c r="F6" t="n">
+        <v>44</v>
+      </c>
+      <c r="G6" t="n">
+        <v>65423</v>
+      </c>
+      <c r="H6" t="n">
+        <v>65018</v>
+      </c>
+      <c r="I6" t="n">
+        <v>750</v>
+      </c>
+      <c r="J6" t="n">
+        <v>63952</v>
+      </c>
+      <c r="K6" t="n">
+        <v>924</v>
+      </c>
+      <c r="L6" t="n">
+        <v>896</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" t="n">
-        <v>25029</v>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>SENSOR_IMU_X</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>{'63812', '69'}</t>
-        </is>
+      <c r="A7" s="1" t="n">
+        <v>55125</v>
+      </c>
+      <c r="B7" t="n">
+        <v>819957</v>
+      </c>
+      <c r="C7" t="n">
+        <v>3245</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8" t="n">
-        <v>25029</v>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>SENSOR_IMU_Y</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>{'654', '582'}</t>
-        </is>
+      <c r="A8" s="1" t="n">
+        <v>55229</v>
+      </c>
+      <c r="D8" t="n">
+        <v>65522</v>
+      </c>
+      <c r="E8" t="n">
+        <v>65510</v>
+      </c>
+      <c r="F8" t="n">
+        <v>65477</v>
+      </c>
+      <c r="G8" t="n">
+        <v>65532</v>
+      </c>
+      <c r="H8" t="n">
+        <v>1089</v>
+      </c>
+      <c r="I8" t="n">
+        <v>164</v>
       </c>
     </row>
     <row r="9">
-      <c r="A9" t="n">
-        <v>25029</v>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>SENSOR_IMU_Z</t>
-        </is>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>{'4564', '7823'}</t>
-        </is>
+      <c r="A9" s="1" t="n">
+        <v>55440</v>
+      </c>
+      <c r="B9" t="n">
+        <v>818682</v>
+      </c>
+      <c r="C9" t="n">
+        <v>3245</v>
+      </c>
+      <c r="D9" t="n">
+        <v>65519</v>
+      </c>
+      <c r="E9" t="n">
+        <v>65477</v>
+      </c>
+      <c r="F9" t="n">
+        <v>65491</v>
+      </c>
+      <c r="G9" t="n">
+        <v>65520</v>
+      </c>
+      <c r="H9" t="n">
+        <v>1155</v>
+      </c>
+      <c r="I9" t="n">
+        <v>159</v>
+      </c>
+      <c r="J9" t="n">
+        <v>65174</v>
+      </c>
+      <c r="K9" t="n">
+        <v>1232</v>
+      </c>
+      <c r="L9" t="n">
+        <v>700</v>
       </c>
     </row>
     <row r="10">
-      <c r="A10" t="n">
-        <v>25029</v>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>SENSOR_MAG_X</t>
-        </is>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>{'64335'}</t>
-        </is>
+      <c r="A10" s="1" t="n">
+        <v>55546</v>
+      </c>
+      <c r="D10" t="n">
+        <v>65516</v>
+      </c>
+      <c r="E10" t="n">
+        <v>65506</v>
       </c>
     </row>
     <row r="11">
-      <c r="A11" t="n">
-        <v>25029</v>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>SENSOR_MAG_Y</t>
-        </is>
-      </c>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>{'502'}</t>
-        </is>
+      <c r="A11" s="1" t="n">
+        <v>70327</v>
+      </c>
+      <c r="B11" t="n">
+        <v>799316</v>
+      </c>
+      <c r="C11" t="n">
+        <v>3141</v>
+      </c>
+      <c r="D11" t="n">
+        <v>22</v>
+      </c>
+      <c r="E11" t="n">
+        <v>15</v>
+      </c>
+      <c r="F11" t="n">
+        <v>65475</v>
+      </c>
+      <c r="G11" t="n">
+        <v>100</v>
+      </c>
+      <c r="H11" t="n">
+        <v>649</v>
+      </c>
+      <c r="I11" t="n">
+        <v>313</v>
+      </c>
+      <c r="J11" t="n">
+        <v>64857</v>
+      </c>
+      <c r="K11" t="n">
+        <v>1531</v>
+      </c>
+      <c r="L11" t="n">
+        <v>65194</v>
       </c>
     </row>
     <row r="12">
-      <c r="A12" t="n">
-        <v>25029</v>
-      </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>SENSOR_MAG_Z</t>
-        </is>
-      </c>
-      <c r="C12" t="inlineStr">
-        <is>
-          <t>{'943'}</t>
-        </is>
+      <c r="A12" s="1" t="n">
+        <v>85426</v>
+      </c>
+      <c r="B12" t="n">
+        <v>1019289</v>
+      </c>
+      <c r="C12" t="n">
+        <v>2806</v>
+      </c>
+      <c r="F12" t="n">
+        <v>6</v>
+      </c>
+      <c r="G12" t="n">
+        <v>65137</v>
+      </c>
+      <c r="H12" t="n">
+        <v>1094</v>
+      </c>
+      <c r="I12" t="n">
+        <v>905</v>
+      </c>
+      <c r="J12" t="n">
+        <v>64876</v>
+      </c>
+      <c r="K12" t="n">
+        <v>824</v>
+      </c>
+      <c r="L12" t="n">
+        <v>64868</v>
       </c>
     </row>
     <row r="13">
-      <c r="A13" t="n">
-        <v>25029</v>
-      </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>SENSOR_BARO</t>
-        </is>
-      </c>
-      <c r="C13" t="inlineStr">
-        <is>
-          <t>{'2175746', '3211'}</t>
-        </is>
+      <c r="A13" s="1" t="n">
+        <v>85532</v>
+      </c>
+      <c r="B13" t="n">
+        <v>1016676</v>
+      </c>
+      <c r="C13" t="n">
+        <v>2804</v>
+      </c>
+      <c r="D13" t="n">
+        <v>65514</v>
+      </c>
+      <c r="E13" t="n">
+        <v>65484</v>
+      </c>
+      <c r="F13" t="n">
+        <v>2</v>
+      </c>
+      <c r="G13" t="n">
+        <v>24</v>
+      </c>
+      <c r="H13" t="n">
+        <v>1053</v>
+      </c>
+      <c r="I13" t="n">
+        <v>940</v>
+      </c>
+      <c r="J13" t="n">
+        <v>64862</v>
+      </c>
+      <c r="K13" t="n">
+        <v>771</v>
+      </c>
+      <c r="L13" t="n">
+        <v>64853</v>
       </c>
     </row>
     <row r="14">
-      <c r="A14" t="n">
-        <v>25029</v>
-      </c>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>SENSOR_BARO</t>
-        </is>
-      </c>
-      <c r="C14" t="inlineStr">
-        <is>
-          <t>{'2175746', '3211'}</t>
-        </is>
+      <c r="A14" s="1" t="n">
+        <v>85743</v>
+      </c>
+      <c r="B14" t="n">
+        <v>1027103</v>
+      </c>
+      <c r="C14" t="n">
+        <v>2803</v>
+      </c>
+      <c r="D14" t="n">
+        <v>65508</v>
+      </c>
+      <c r="E14" t="n">
+        <v>65447</v>
+      </c>
+      <c r="F14" t="n">
+        <v>65526</v>
+      </c>
+      <c r="G14" t="n">
+        <v>65272</v>
+      </c>
+      <c r="H14" t="n">
+        <v>919</v>
+      </c>
+      <c r="I14" t="n">
+        <v>905</v>
+      </c>
+      <c r="J14" t="n">
+        <v>64823</v>
+      </c>
+      <c r="K14" t="n">
+        <v>688</v>
+      </c>
+      <c r="L14" t="n">
+        <v>64854</v>
       </c>
     </row>
     <row r="15">
-      <c r="A15" t="n">
-        <v>39917</v>
-      </c>
-      <c r="B15" t="inlineStr">
-        <is>
-          <t>SENSOR_IMU_X</t>
-        </is>
-      </c>
-      <c r="C15" t="inlineStr">
-        <is>
-          <t>{'27', '65499'}</t>
-        </is>
+      <c r="A15" s="1" t="n">
+        <v>100738</v>
+      </c>
+      <c r="B15" t="n">
+        <v>1487106</v>
+      </c>
+      <c r="C15" t="n">
+        <v>2313</v>
+      </c>
+      <c r="F15" t="n">
+        <v>17</v>
+      </c>
+      <c r="G15" t="n">
+        <v>65202</v>
+      </c>
+      <c r="H15" t="n">
+        <v>6</v>
+      </c>
+      <c r="I15" t="n">
+        <v>1792</v>
+      </c>
+      <c r="J15" t="n">
+        <v>64201</v>
+      </c>
+      <c r="K15" t="n">
+        <v>1013</v>
+      </c>
+      <c r="L15" t="n">
+        <v>64799</v>
       </c>
     </row>
     <row r="16">
-      <c r="A16" t="n">
-        <v>39917</v>
-      </c>
-      <c r="B16" t="inlineStr">
-        <is>
-          <t>SENSOR_IMU_Y</t>
-        </is>
-      </c>
-      <c r="C16" t="inlineStr">
-        <is>
-          <t>{'65493', '21'}</t>
-        </is>
+      <c r="A16" s="1" t="n">
+        <v>100950</v>
+      </c>
+      <c r="B16" t="n">
+        <v>1494342</v>
+      </c>
+      <c r="C16" t="n">
+        <v>2308</v>
+      </c>
+      <c r="D16" t="n">
+        <v>30</v>
+      </c>
+      <c r="E16" t="n">
+        <v>79</v>
+      </c>
+      <c r="F16" t="n">
+        <v>9</v>
+      </c>
+      <c r="G16" t="n">
+        <v>65403</v>
+      </c>
+      <c r="H16" t="n">
+        <v>116</v>
+      </c>
+      <c r="I16" t="n">
+        <v>1892</v>
+      </c>
+      <c r="J16" t="n">
+        <v>64220</v>
+      </c>
+      <c r="K16" t="n">
+        <v>1003</v>
+      </c>
+      <c r="L16" t="n">
+        <v>64664</v>
       </c>
     </row>
     <row r="17">
-      <c r="A17" t="n">
-        <v>39917</v>
-      </c>
-      <c r="B17" t="inlineStr">
-        <is>
-          <t>SENSOR_IMU_Z</t>
-        </is>
-      </c>
-      <c r="C17" t="inlineStr">
-        <is>
-          <t>{'64884', '806'}</t>
-        </is>
+      <c r="A17" s="1" t="n">
+        <v>115945</v>
+      </c>
+      <c r="B17" t="n">
+        <v>2161418</v>
+      </c>
+      <c r="C17" t="n">
+        <v>2105</v>
+      </c>
+      <c r="H17" t="n">
+        <v>64991</v>
+      </c>
+      <c r="I17" t="n">
+        <v>2021</v>
+      </c>
+      <c r="J17" t="n">
+        <v>64393</v>
+      </c>
+      <c r="K17" t="n">
+        <v>1087</v>
+      </c>
+      <c r="L17" t="n">
+        <v>64771</v>
       </c>
     </row>
     <row r="18">
-      <c r="A18" t="n">
-        <v>40237</v>
-      </c>
-      <c r="B18" t="inlineStr">
-        <is>
-          <t>SENSOR_IMU_X</t>
-        </is>
-      </c>
-      <c r="C18" t="inlineStr">
-        <is>
-          <t>{'65500', '65535'}</t>
-        </is>
+      <c r="A18" s="1" t="n">
+        <v>116260</v>
+      </c>
+      <c r="B18" t="n">
+        <v>2158255</v>
+      </c>
+      <c r="C18" t="n">
+        <v>2106</v>
+      </c>
+      <c r="D18" t="n">
+        <v>61</v>
+      </c>
+      <c r="E18" t="n">
+        <v>64950</v>
+      </c>
+      <c r="F18" t="n">
+        <v>65475</v>
+      </c>
+      <c r="G18" t="n">
+        <v>65421</v>
+      </c>
+      <c r="H18" t="n">
+        <v>64988</v>
+      </c>
+      <c r="I18" t="n">
+        <v>2146</v>
+      </c>
+      <c r="J18" t="n">
+        <v>64367</v>
+      </c>
+      <c r="K18" t="n">
+        <v>1084</v>
+      </c>
+      <c r="L18" t="n">
+        <v>64759</v>
       </c>
     </row>
     <row r="19">
-      <c r="A19" t="n">
-        <v>40237</v>
-      </c>
-      <c r="B19" t="inlineStr">
-        <is>
-          <t>SENSOR_IMU_Y</t>
-        </is>
-      </c>
-      <c r="C19" t="inlineStr">
-        <is>
-          <t>{'44', '65423'}</t>
-        </is>
+      <c r="A19" s="1" t="n">
+        <v>116366</v>
+      </c>
+      <c r="D19" t="n">
+        <v>24</v>
+      </c>
+      <c r="E19" t="n">
+        <v>64644</v>
+      </c>
+      <c r="F19" t="n">
+        <v>65531</v>
+      </c>
+      <c r="G19" t="n">
+        <v>31</v>
+      </c>
+      <c r="H19" t="n">
+        <v>64817</v>
+      </c>
+      <c r="I19" t="n">
+        <v>2256</v>
+      </c>
+      <c r="J19" t="n">
+        <v>64359</v>
+      </c>
+      <c r="K19" t="n">
+        <v>1070</v>
       </c>
     </row>
     <row r="20">
-      <c r="A20" t="n">
-        <v>40237</v>
-      </c>
-      <c r="B20" t="inlineStr">
-        <is>
-          <t>SENSOR_IMU_Z</t>
-        </is>
-      </c>
-      <c r="C20" t="inlineStr">
-        <is>
-          <t>{'65018', '750'}</t>
-        </is>
+      <c r="A20" s="1" t="n">
+        <v>131253</v>
+      </c>
+      <c r="B20" t="n">
+        <v>2977769</v>
+      </c>
+      <c r="C20" t="n">
+        <v>2088</v>
+      </c>
+      <c r="D20" t="n">
+        <v>57</v>
+      </c>
+      <c r="E20" t="n">
+        <v>64640</v>
+      </c>
+      <c r="F20" t="n">
+        <v>65535</v>
+      </c>
+      <c r="G20" t="n">
+        <v>65244</v>
+      </c>
+      <c r="H20" t="n">
+        <v>63759</v>
+      </c>
+      <c r="I20" t="n">
+        <v>2266</v>
+      </c>
+      <c r="J20" t="n">
+        <v>64641</v>
+      </c>
+      <c r="K20" t="n">
+        <v>1118</v>
+      </c>
+      <c r="L20" t="n">
+        <v>64793</v>
       </c>
     </row>
     <row r="21">
-      <c r="A21" t="n">
-        <v>40237</v>
-      </c>
-      <c r="B21" t="inlineStr">
-        <is>
-          <t>SENSOR_MAG_X</t>
-        </is>
-      </c>
-      <c r="C21" t="inlineStr">
-        <is>
-          <t>{'63952'}</t>
-        </is>
+      <c r="A21" s="1" t="n">
+        <v>131569</v>
+      </c>
+      <c r="D21" t="n">
+        <v>52</v>
+      </c>
+      <c r="E21" t="n">
+        <v>65063</v>
+      </c>
+      <c r="F21" t="n">
+        <v>96</v>
+      </c>
+      <c r="G21" t="n">
+        <v>104</v>
+      </c>
+      <c r="H21" t="n">
+        <v>63520</v>
+      </c>
+      <c r="I21" t="n">
+        <v>2461</v>
+      </c>
+      <c r="J21" t="n">
+        <v>64425</v>
+      </c>
+      <c r="K21" t="n">
+        <v>1136</v>
+      </c>
+      <c r="L21" t="n">
+        <v>64790</v>
       </c>
     </row>
     <row r="22">
-      <c r="A22" t="n">
-        <v>40237</v>
-      </c>
-      <c r="B22" t="inlineStr">
-        <is>
-          <t>SENSOR_MAG_Y</t>
-        </is>
-      </c>
-      <c r="C22" t="inlineStr">
-        <is>
-          <t>{'924'}</t>
-        </is>
+      <c r="A22" s="1" t="n">
+        <v>146457</v>
+      </c>
+      <c r="B22" t="n">
+        <v>3912278</v>
+      </c>
+      <c r="C22" t="n">
+        <v>2174</v>
+      </c>
+      <c r="D22" t="n">
+        <v>65469</v>
+      </c>
+      <c r="E22" t="n">
+        <v>65062</v>
+      </c>
+      <c r="F22" t="n">
+        <v>118</v>
+      </c>
+      <c r="G22" t="n">
+        <v>65304</v>
+      </c>
+      <c r="H22" t="n">
+        <v>64204</v>
+      </c>
+      <c r="I22" t="n">
+        <v>2241</v>
+      </c>
+      <c r="J22" t="n">
+        <v>64209</v>
+      </c>
+      <c r="K22" t="n">
+        <v>918</v>
+      </c>
+      <c r="L22" t="n">
+        <v>64761</v>
       </c>
     </row>
     <row r="23">
-      <c r="A23" t="n">
-        <v>40237</v>
-      </c>
-      <c r="B23" t="inlineStr">
-        <is>
-          <t>SENSOR_MAG_Z</t>
-        </is>
-      </c>
-      <c r="C23" t="inlineStr">
-        <is>
-          <t>{'896'}</t>
-        </is>
+      <c r="A23" s="1" t="n">
+        <v>146563</v>
+      </c>
+      <c r="D23" t="n">
+        <v>446</v>
+      </c>
+      <c r="E23" t="n">
+        <v>65401</v>
       </c>
     </row>
     <row r="24">
-      <c r="A24" t="n">
-        <v>40237</v>
-      </c>
-      <c r="B24" t="inlineStr">
-        <is>
-          <t>SENSOR_BARO</t>
-        </is>
-      </c>
-      <c r="C24" t="inlineStr">
-        <is>
-          <t>{'1115428', '3258'}</t>
-        </is>
-      </c>
-    </row>
-    <row r="25">
-      <c r="A25" t="n">
-        <v>55125</v>
-      </c>
-      <c r="B25" t="inlineStr">
-        <is>
-          <t>SENSOR_BARO</t>
-        </is>
-      </c>
-      <c r="C25" t="inlineStr">
-        <is>
-          <t>{'3245', '819957'}</t>
-        </is>
-      </c>
-    </row>
-    <row r="26">
-      <c r="A26" t="n">
-        <v>55229</v>
-      </c>
-      <c r="B26" t="inlineStr">
-        <is>
-          <t>SENSOR_IMU_X</t>
-        </is>
-      </c>
-      <c r="C26" t="inlineStr">
-        <is>
-          <t>{'65510', '65522'}</t>
-        </is>
-      </c>
-    </row>
-    <row r="27">
-      <c r="A27" t="n">
-        <v>55229</v>
-      </c>
-      <c r="B27" t="inlineStr">
-        <is>
-          <t>SENSOR_IMU_Y</t>
-        </is>
-      </c>
-      <c r="C27" t="inlineStr">
-        <is>
-          <t>{'65532', '65477'}</t>
-        </is>
-      </c>
-    </row>
-    <row r="28">
-      <c r="A28" t="n">
-        <v>55229</v>
-      </c>
-      <c r="B28" t="inlineStr">
-        <is>
-          <t>SENSOR_IMU_Z</t>
-        </is>
-      </c>
-      <c r="C28" t="inlineStr">
-        <is>
-          <t>{'1089', '164'}</t>
-        </is>
-      </c>
-    </row>
-    <row r="29">
-      <c r="A29" t="n">
-        <v>55440</v>
-      </c>
-      <c r="B29" t="inlineStr">
-        <is>
-          <t>SENSOR_IMU_X</t>
-        </is>
-      </c>
-      <c r="C29" t="inlineStr">
-        <is>
-          <t>{'65519', '65477'}</t>
-        </is>
-      </c>
-    </row>
-    <row r="30">
-      <c r="A30" t="n">
-        <v>55440</v>
-      </c>
-      <c r="B30" t="inlineStr">
-        <is>
-          <t>SENSOR_IMU_Y</t>
-        </is>
-      </c>
-      <c r="C30" t="inlineStr">
-        <is>
-          <t>{'65491', '65520'}</t>
-        </is>
-      </c>
-    </row>
-    <row r="31">
-      <c r="A31" t="n">
-        <v>55440</v>
-      </c>
-      <c r="B31" t="inlineStr">
-        <is>
-          <t>SENSOR_IMU_Z</t>
-        </is>
-      </c>
-      <c r="C31" t="inlineStr">
-        <is>
-          <t>{'159', '1155'}</t>
-        </is>
-      </c>
-    </row>
-    <row r="32">
-      <c r="A32" t="n">
-        <v>55440</v>
-      </c>
-      <c r="B32" t="inlineStr">
-        <is>
-          <t>SENSOR_MAG_X</t>
-        </is>
-      </c>
-      <c r="C32" t="inlineStr">
-        <is>
-          <t>{'65174'}</t>
-        </is>
-      </c>
-    </row>
-    <row r="33">
-      <c r="A33" t="n">
-        <v>55440</v>
-      </c>
-      <c r="B33" t="inlineStr">
-        <is>
-          <t>SENSOR_MAG_Y</t>
-        </is>
-      </c>
-      <c r="C33" t="inlineStr">
-        <is>
-          <t>{'1232'}</t>
-        </is>
-      </c>
-    </row>
-    <row r="34">
-      <c r="A34" t="n">
-        <v>55440</v>
-      </c>
-      <c r="B34" t="inlineStr">
-        <is>
-          <t>SENSOR_MAG_Z</t>
-        </is>
-      </c>
-      <c r="C34" t="inlineStr">
-        <is>
-          <t>{'700'}</t>
-        </is>
-      </c>
-    </row>
-    <row r="35">
-      <c r="A35" t="n">
-        <v>55440</v>
-      </c>
-      <c r="B35" t="inlineStr">
-        <is>
-          <t>SENSOR_BARO</t>
-        </is>
-      </c>
-      <c r="C35" t="inlineStr">
-        <is>
-          <t>{'3245', '818682'}</t>
-        </is>
-      </c>
-    </row>
-    <row r="36">
-      <c r="A36" t="n">
-        <v>55546</v>
-      </c>
-      <c r="B36" t="inlineStr">
-        <is>
-          <t>SENSOR_IMU_X</t>
-        </is>
-      </c>
-      <c r="C36" t="inlineStr">
-        <is>
-          <t>{'65506', '65516'}</t>
-        </is>
-      </c>
-    </row>
-    <row r="37">
-      <c r="A37" t="n">
-        <v>70327</v>
-      </c>
-      <c r="B37" t="inlineStr">
-        <is>
-          <t>SENSOR_IMU_X</t>
-        </is>
-      </c>
-      <c r="C37" t="inlineStr">
-        <is>
-          <t>{'22', '15'}</t>
-        </is>
-      </c>
-    </row>
-    <row r="38">
-      <c r="A38" t="n">
-        <v>70327</v>
-      </c>
-      <c r="B38" t="inlineStr">
-        <is>
-          <t>SENSOR_IMU_Y</t>
-        </is>
-      </c>
-      <c r="C38" t="inlineStr">
-        <is>
-          <t>{'65475', '100'}</t>
-        </is>
-      </c>
-    </row>
-    <row r="39">
-      <c r="A39" t="n">
-        <v>70327</v>
-      </c>
-      <c r="B39" t="inlineStr">
-        <is>
-          <t>SENSOR_IMU_Z</t>
-        </is>
-      </c>
-      <c r="C39" t="inlineStr">
-        <is>
-          <t>{'313', '649'}</t>
-        </is>
-      </c>
-    </row>
-    <row r="40">
-      <c r="A40" t="n">
-        <v>70327</v>
-      </c>
-      <c r="B40" t="inlineStr">
-        <is>
-          <t>SENSOR_MAG_X</t>
-        </is>
-      </c>
-      <c r="C40" t="inlineStr">
-        <is>
-          <t>{'64857'}</t>
-        </is>
-      </c>
-    </row>
-    <row r="41">
-      <c r="A41" t="n">
-        <v>70327</v>
-      </c>
-      <c r="B41" t="inlineStr">
-        <is>
-          <t>SENSOR_MAG_Y</t>
-        </is>
-      </c>
-      <c r="C41" t="inlineStr">
-        <is>
-          <t>{'1531'}</t>
-        </is>
-      </c>
-    </row>
-    <row r="42">
-      <c r="A42" t="n">
-        <v>70327</v>
-      </c>
-      <c r="B42" t="inlineStr">
-        <is>
-          <t>SENSOR_MAG_Z</t>
-        </is>
-      </c>
-      <c r="C42" t="inlineStr">
-        <is>
-          <t>{'65194'}</t>
-        </is>
-      </c>
-    </row>
-    <row r="43">
-      <c r="A43" t="n">
-        <v>70327</v>
-      </c>
-      <c r="B43" t="inlineStr">
-        <is>
-          <t>SENSOR_BARO</t>
-        </is>
-      </c>
-      <c r="C43" t="inlineStr">
-        <is>
-          <t>{'799316', '3141'}</t>
-        </is>
-      </c>
-    </row>
-    <row r="44">
-      <c r="A44" t="n">
-        <v>85426</v>
-      </c>
-      <c r="B44" t="inlineStr">
-        <is>
-          <t>SENSOR_IMU_Y</t>
-        </is>
-      </c>
-      <c r="C44" t="inlineStr">
-        <is>
-          <t>{'65137', '6'}</t>
-        </is>
-      </c>
-    </row>
-    <row r="45">
-      <c r="A45" t="n">
-        <v>85426</v>
-      </c>
-      <c r="B45" t="inlineStr">
-        <is>
-          <t>SENSOR_IMU_Z</t>
-        </is>
-      </c>
-      <c r="C45" t="inlineStr">
-        <is>
-          <t>{'1094', '905'}</t>
-        </is>
-      </c>
-    </row>
-    <row r="46">
-      <c r="A46" t="n">
-        <v>85426</v>
-      </c>
-      <c r="B46" t="inlineStr">
-        <is>
-          <t>SENSOR_MAG_X</t>
-        </is>
-      </c>
-      <c r="C46" t="inlineStr">
-        <is>
-          <t>{'64876'}</t>
-        </is>
-      </c>
-    </row>
-    <row r="47">
-      <c r="A47" t="n">
-        <v>85426</v>
-      </c>
-      <c r="B47" t="inlineStr">
-        <is>
-          <t>SENSOR_MAG_Y</t>
-        </is>
-      </c>
-      <c r="C47" t="inlineStr">
-        <is>
-          <t>{'824'}</t>
-        </is>
-      </c>
-    </row>
-    <row r="48">
-      <c r="A48" t="n">
-        <v>85426</v>
-      </c>
-      <c r="B48" t="inlineStr">
-        <is>
-          <t>SENSOR_MAG_Z</t>
-        </is>
-      </c>
-      <c r="C48" t="inlineStr">
-        <is>
-          <t>{'64868'}</t>
-        </is>
-      </c>
-    </row>
-    <row r="49">
-      <c r="A49" t="n">
-        <v>85426</v>
-      </c>
-      <c r="B49" t="inlineStr">
-        <is>
-          <t>SENSOR_BARO</t>
-        </is>
-      </c>
-      <c r="C49" t="inlineStr">
-        <is>
-          <t>{'1019289', '2806'}</t>
-        </is>
-      </c>
-    </row>
-    <row r="50">
-      <c r="A50" t="n">
-        <v>85532</v>
-      </c>
-      <c r="B50" t="inlineStr">
-        <is>
-          <t>SENSOR_IMU_X</t>
-        </is>
-      </c>
-      <c r="C50" t="inlineStr">
-        <is>
-          <t>{'65484', '65514'}</t>
-        </is>
-      </c>
-    </row>
-    <row r="51">
-      <c r="A51" t="n">
-        <v>85532</v>
-      </c>
-      <c r="B51" t="inlineStr">
-        <is>
-          <t>SENSOR_IMU_Y</t>
-        </is>
-      </c>
-      <c r="C51" t="inlineStr">
-        <is>
-          <t>{'24', '2'}</t>
-        </is>
-      </c>
-    </row>
-    <row r="52">
-      <c r="A52" t="n">
-        <v>85532</v>
-      </c>
-      <c r="B52" t="inlineStr">
-        <is>
-          <t>SENSOR_IMU_Z</t>
-        </is>
-      </c>
-      <c r="C52" t="inlineStr">
-        <is>
-          <t>{'1053', '940'}</t>
-        </is>
-      </c>
-    </row>
-    <row r="53">
-      <c r="A53" t="n">
-        <v>85532</v>
-      </c>
-      <c r="B53" t="inlineStr">
-        <is>
-          <t>SENSOR_MAG_X</t>
-        </is>
-      </c>
-      <c r="C53" t="inlineStr">
-        <is>
-          <t>{'64862'}</t>
-        </is>
-      </c>
-    </row>
-    <row r="54">
-      <c r="A54" t="n">
-        <v>85532</v>
-      </c>
-      <c r="B54" t="inlineStr">
-        <is>
-          <t>SENSOR_MAG_Y</t>
-        </is>
-      </c>
-      <c r="C54" t="inlineStr">
-        <is>
-          <t>{'771'}</t>
-        </is>
-      </c>
-    </row>
-    <row r="55">
-      <c r="A55" t="n">
-        <v>85532</v>
-      </c>
-      <c r="B55" t="inlineStr">
-        <is>
-          <t>SENSOR_MAG_Z</t>
-        </is>
-      </c>
-      <c r="C55" t="inlineStr">
-        <is>
-          <t>{'64853'}</t>
-        </is>
-      </c>
-    </row>
-    <row r="56">
-      <c r="A56" t="n">
-        <v>85532</v>
-      </c>
-      <c r="B56" t="inlineStr">
-        <is>
-          <t>SENSOR_BARO</t>
-        </is>
-      </c>
-      <c r="C56" t="inlineStr">
-        <is>
-          <t>{'1016676', '2804'}</t>
-        </is>
-      </c>
-    </row>
-    <row r="57">
-      <c r="A57" t="n">
-        <v>85743</v>
-      </c>
-      <c r="B57" t="inlineStr">
-        <is>
-          <t>SENSOR_IMU_X</t>
-        </is>
-      </c>
-      <c r="C57" t="inlineStr">
-        <is>
-          <t>{'65508', '65447'}</t>
-        </is>
-      </c>
-    </row>
-    <row r="58">
-      <c r="A58" t="n">
-        <v>85743</v>
-      </c>
-      <c r="B58" t="inlineStr">
-        <is>
-          <t>SENSOR_IMU_Y</t>
-        </is>
-      </c>
-      <c r="C58" t="inlineStr">
-        <is>
-          <t>{'65526', '65272'}</t>
-        </is>
-      </c>
-    </row>
-    <row r="59">
-      <c r="A59" t="n">
-        <v>85743</v>
-      </c>
-      <c r="B59" t="inlineStr">
-        <is>
-          <t>SENSOR_IMU_Z</t>
-        </is>
-      </c>
-      <c r="C59" t="inlineStr">
-        <is>
-          <t>{'919', '905'}</t>
-        </is>
-      </c>
-    </row>
-    <row r="60">
-      <c r="A60" t="n">
-        <v>85743</v>
-      </c>
-      <c r="B60" t="inlineStr">
-        <is>
-          <t>SENSOR_MAG_X</t>
-        </is>
-      </c>
-      <c r="C60" t="inlineStr">
-        <is>
-          <t>{'64823'}</t>
-        </is>
-      </c>
-    </row>
-    <row r="61">
-      <c r="A61" t="n">
-        <v>85743</v>
-      </c>
-      <c r="B61" t="inlineStr">
-        <is>
-          <t>SENSOR_MAG_Y</t>
-        </is>
-      </c>
-      <c r="C61" t="inlineStr">
-        <is>
-          <t>{'688'}</t>
-        </is>
-      </c>
-    </row>
-    <row r="62">
-      <c r="A62" t="n">
-        <v>85743</v>
-      </c>
-      <c r="B62" t="inlineStr">
-        <is>
-          <t>SENSOR_MAG_Z</t>
-        </is>
-      </c>
-      <c r="C62" t="inlineStr">
-        <is>
-          <t>{'64854'}</t>
-        </is>
-      </c>
-    </row>
-    <row r="63">
-      <c r="A63" t="n">
-        <v>85743</v>
-      </c>
-      <c r="B63" t="inlineStr">
-        <is>
-          <t>SENSOR_BARO</t>
-        </is>
-      </c>
-      <c r="C63" t="inlineStr">
-        <is>
-          <t>{'2803', '1027103'}</t>
-        </is>
-      </c>
-    </row>
-    <row r="64">
-      <c r="A64" t="n">
-        <v>100738</v>
-      </c>
-      <c r="B64" t="inlineStr">
-        <is>
-          <t>SENSOR_IMU_Y</t>
-        </is>
-      </c>
-      <c r="C64" t="inlineStr">
-        <is>
-          <t>{'17', '65202'}</t>
-        </is>
-      </c>
-    </row>
-    <row r="65">
-      <c r="A65" t="n">
-        <v>100738</v>
-      </c>
-      <c r="B65" t="inlineStr">
-        <is>
-          <t>SENSOR_IMU_Z</t>
-        </is>
-      </c>
-      <c r="C65" t="inlineStr">
-        <is>
-          <t>{'6', '1792'}</t>
-        </is>
-      </c>
-    </row>
-    <row r="66">
-      <c r="A66" t="n">
-        <v>100738</v>
-      </c>
-      <c r="B66" t="inlineStr">
-        <is>
-          <t>SENSOR_MAG_X</t>
-        </is>
-      </c>
-      <c r="C66" t="inlineStr">
-        <is>
-          <t>{'64201'}</t>
-        </is>
-      </c>
-    </row>
-    <row r="67">
-      <c r="A67" t="n">
-        <v>100738</v>
-      </c>
-      <c r="B67" t="inlineStr">
-        <is>
-          <t>SENSOR_MAG_Y</t>
-        </is>
-      </c>
-      <c r="C67" t="inlineStr">
-        <is>
-          <t>{'1013'}</t>
-        </is>
-      </c>
-    </row>
-    <row r="68">
-      <c r="A68" t="n">
-        <v>100738</v>
-      </c>
-      <c r="B68" t="inlineStr">
-        <is>
-          <t>SENSOR_MAG_Z</t>
-        </is>
-      </c>
-      <c r="C68" t="inlineStr">
-        <is>
-          <t>{'64799'}</t>
-        </is>
-      </c>
-    </row>
-    <row r="69">
-      <c r="A69" t="n">
-        <v>100738</v>
-      </c>
-      <c r="B69" t="inlineStr">
-        <is>
-          <t>SENSOR_BARO</t>
-        </is>
-      </c>
-      <c r="C69" t="inlineStr">
-        <is>
-          <t>{'2313', '1487106'}</t>
-        </is>
-      </c>
-    </row>
-    <row r="70">
-      <c r="A70" t="n">
-        <v>100950</v>
-      </c>
-      <c r="B70" t="inlineStr">
-        <is>
-          <t>SENSOR_IMU_X</t>
-        </is>
-      </c>
-      <c r="C70" t="inlineStr">
-        <is>
-          <t>{'30', '79'}</t>
-        </is>
-      </c>
-    </row>
-    <row r="71">
-      <c r="A71" t="n">
-        <v>100950</v>
-      </c>
-      <c r="B71" t="inlineStr">
-        <is>
-          <t>SENSOR_IMU_Y</t>
-        </is>
-      </c>
-      <c r="C71" t="inlineStr">
-        <is>
-          <t>{'9', '65403'}</t>
-        </is>
-      </c>
-    </row>
-    <row r="72">
-      <c r="A72" t="n">
-        <v>100950</v>
-      </c>
-      <c r="B72" t="inlineStr">
-        <is>
-          <t>SENSOR_IMU_Z</t>
-        </is>
-      </c>
-      <c r="C72" t="inlineStr">
-        <is>
-          <t>{'1892', '116'}</t>
-        </is>
-      </c>
-    </row>
-    <row r="73">
-      <c r="A73" t="n">
-        <v>100950</v>
-      </c>
-      <c r="B73" t="inlineStr">
-        <is>
-          <t>SENSOR_MAG_X</t>
-        </is>
-      </c>
-      <c r="C73" t="inlineStr">
-        <is>
-          <t>{'64220'}</t>
-        </is>
-      </c>
-    </row>
-    <row r="74">
-      <c r="A74" t="n">
-        <v>100950</v>
-      </c>
-      <c r="B74" t="inlineStr">
-        <is>
-          <t>SENSOR_MAG_Y</t>
-        </is>
-      </c>
-      <c r="C74" t="inlineStr">
-        <is>
-          <t>{'1003'}</t>
-        </is>
-      </c>
-    </row>
-    <row r="75">
-      <c r="A75" t="n">
-        <v>100950</v>
-      </c>
-      <c r="B75" t="inlineStr">
-        <is>
-          <t>SENSOR_MAG_Y</t>
-        </is>
-      </c>
-      <c r="C75" t="inlineStr">
-        <is>
-          <t>{'1003'}</t>
-        </is>
-      </c>
-    </row>
-    <row r="76">
-      <c r="A76" t="n">
-        <v>100950</v>
-      </c>
-      <c r="B76" t="inlineStr">
-        <is>
-          <t>SENSOR_MAG_Z</t>
-        </is>
-      </c>
-      <c r="C76" t="inlineStr">
-        <is>
-          <t>{'64664'}</t>
-        </is>
-      </c>
-    </row>
-    <row r="77">
-      <c r="A77" t="n">
-        <v>100950</v>
-      </c>
-      <c r="B77" t="inlineStr">
-        <is>
-          <t>SENSOR_BARO</t>
-        </is>
-      </c>
-      <c r="C77" t="inlineStr">
-        <is>
-          <t>{'1494342', '2308'}</t>
-        </is>
-      </c>
-    </row>
-    <row r="78">
-      <c r="A78" t="n">
-        <v>115945</v>
-      </c>
-      <c r="B78" t="inlineStr">
-        <is>
-          <t>SENSOR_IMU_Z</t>
-        </is>
-      </c>
-      <c r="C78" t="inlineStr">
-        <is>
-          <t>{'64991', '2021'}</t>
-        </is>
-      </c>
-    </row>
-    <row r="79">
-      <c r="A79" t="n">
-        <v>115945</v>
-      </c>
-      <c r="B79" t="inlineStr">
-        <is>
-          <t>SENSOR_MAG_X</t>
-        </is>
-      </c>
-      <c r="C79" t="inlineStr">
-        <is>
-          <t>{'64393'}</t>
-        </is>
-      </c>
-    </row>
-    <row r="80">
-      <c r="A80" t="n">
-        <v>115945</v>
-      </c>
-      <c r="B80" t="inlineStr">
-        <is>
-          <t>SENSOR_MAG_Y</t>
-        </is>
-      </c>
-      <c r="C80" t="inlineStr">
-        <is>
-          <t>{'1087'}</t>
-        </is>
-      </c>
-    </row>
-    <row r="81">
-      <c r="A81" t="n">
-        <v>115945</v>
-      </c>
-      <c r="B81" t="inlineStr">
-        <is>
-          <t>SENSOR_MAG_Z</t>
-        </is>
-      </c>
-      <c r="C81" t="inlineStr">
-        <is>
-          <t>{'64771'}</t>
-        </is>
-      </c>
-    </row>
-    <row r="82">
-      <c r="A82" t="n">
-        <v>115945</v>
-      </c>
-      <c r="B82" t="inlineStr">
-        <is>
-          <t>SENSOR_BARO</t>
-        </is>
-      </c>
-      <c r="C82" t="inlineStr">
-        <is>
-          <t>{'2105', '2161418'}</t>
-        </is>
-      </c>
-    </row>
-    <row r="83">
-      <c r="A83" t="n">
-        <v>116260</v>
-      </c>
-      <c r="B83" t="inlineStr">
-        <is>
-          <t>SENSOR_IMU_X</t>
-        </is>
-      </c>
-      <c r="C83" t="inlineStr">
-        <is>
-          <t>{'64950', '61'}</t>
-        </is>
-      </c>
-    </row>
-    <row r="84">
-      <c r="A84" t="n">
-        <v>116260</v>
-      </c>
-      <c r="B84" t="inlineStr">
-        <is>
-          <t>SENSOR_IMU_Y</t>
-        </is>
-      </c>
-      <c r="C84" t="inlineStr">
-        <is>
-          <t>{'65421', '65475'}</t>
-        </is>
-      </c>
-    </row>
-    <row r="85">
-      <c r="A85" t="n">
-        <v>116260</v>
-      </c>
-      <c r="B85" t="inlineStr">
-        <is>
-          <t>SENSOR_IMU_Z</t>
-        </is>
-      </c>
-      <c r="C85" t="inlineStr">
-        <is>
-          <t>{'2146', '64988'}</t>
-        </is>
-      </c>
-    </row>
-    <row r="86">
-      <c r="A86" t="n">
-        <v>116260</v>
-      </c>
-      <c r="B86" t="inlineStr">
-        <is>
-          <t>SENSOR_MAG_X</t>
-        </is>
-      </c>
-      <c r="C86" t="inlineStr">
-        <is>
-          <t>{'64367'}</t>
-        </is>
-      </c>
-    </row>
-    <row r="87">
-      <c r="A87" t="n">
-        <v>116260</v>
-      </c>
-      <c r="B87" t="inlineStr">
-        <is>
-          <t>SENSOR_MAG_Y</t>
-        </is>
-      </c>
-      <c r="C87" t="inlineStr">
-        <is>
-          <t>{'1084'}</t>
-        </is>
-      </c>
-    </row>
-    <row r="88">
-      <c r="A88" t="n">
-        <v>116260</v>
-      </c>
-      <c r="B88" t="inlineStr">
-        <is>
-          <t>SENSOR_MAG_Z</t>
-        </is>
-      </c>
-      <c r="C88" t="inlineStr">
-        <is>
-          <t>{'64759'}</t>
-        </is>
-      </c>
-    </row>
-    <row r="89">
-      <c r="A89" t="n">
-        <v>116260</v>
-      </c>
-      <c r="B89" t="inlineStr">
-        <is>
-          <t>SENSOR_BARO</t>
-        </is>
-      </c>
-      <c r="C89" t="inlineStr">
-        <is>
-          <t>{'2106', '2158255'}</t>
-        </is>
-      </c>
-    </row>
-    <row r="90">
-      <c r="A90" t="n">
-        <v>116366</v>
-      </c>
-      <c r="B90" t="inlineStr">
-        <is>
-          <t>SENSOR_IMU_X</t>
-        </is>
-      </c>
-      <c r="C90" t="inlineStr">
-        <is>
-          <t>{'64644', '24'}</t>
-        </is>
-      </c>
-    </row>
-    <row r="91">
-      <c r="A91" t="n">
-        <v>116366</v>
-      </c>
-      <c r="B91" t="inlineStr">
-        <is>
-          <t>SENSOR_IMU_Y</t>
-        </is>
-      </c>
-      <c r="C91" t="inlineStr">
-        <is>
-          <t>{'65531', '31'}</t>
-        </is>
-      </c>
-    </row>
-    <row r="92">
-      <c r="A92" t="n">
-        <v>116366</v>
-      </c>
-      <c r="B92" t="inlineStr">
-        <is>
-          <t>SENSOR_IMU_Z</t>
-        </is>
-      </c>
-      <c r="C92" t="inlineStr">
-        <is>
-          <t>{'64817', '2256'}</t>
-        </is>
-      </c>
-    </row>
-    <row r="93">
-      <c r="A93" t="n">
-        <v>116366</v>
-      </c>
-      <c r="B93" t="inlineStr">
-        <is>
-          <t>SENSOR_MAG_X</t>
-        </is>
-      </c>
-      <c r="C93" t="inlineStr">
-        <is>
-          <t>{'64359'}</t>
-        </is>
-      </c>
-    </row>
-    <row r="94">
-      <c r="A94" t="n">
-        <v>116366</v>
-      </c>
-      <c r="B94" t="inlineStr">
-        <is>
-          <t>SENSOR_MAG_Y</t>
-        </is>
-      </c>
-      <c r="C94" t="inlineStr">
-        <is>
-          <t>{'1070'}</t>
-        </is>
-      </c>
-    </row>
-    <row r="95">
-      <c r="A95" t="n">
-        <v>131253</v>
-      </c>
-      <c r="B95" t="inlineStr">
-        <is>
-          <t>SENSOR_IMU_X</t>
-        </is>
-      </c>
-      <c r="C95" t="inlineStr">
-        <is>
-          <t>{'64640', '57'}</t>
-        </is>
-      </c>
-    </row>
-    <row r="96">
-      <c r="A96" t="n">
-        <v>131253</v>
-      </c>
-      <c r="B96" t="inlineStr">
-        <is>
-          <t>SENSOR_IMU_Y</t>
-        </is>
-      </c>
-      <c r="C96" t="inlineStr">
-        <is>
-          <t>{'65244', '65535'}</t>
-        </is>
-      </c>
-    </row>
-    <row r="97">
-      <c r="A97" t="n">
-        <v>131253</v>
-      </c>
-      <c r="B97" t="inlineStr">
-        <is>
-          <t>SENSOR_IMU_Z</t>
-        </is>
-      </c>
-      <c r="C97" t="inlineStr">
-        <is>
-          <t>{'63759', '2266'}</t>
-        </is>
-      </c>
-    </row>
-    <row r="98">
-      <c r="A98" t="n">
-        <v>131253</v>
-      </c>
-      <c r="B98" t="inlineStr">
-        <is>
-          <t>SENSOR_MAG_X</t>
-        </is>
-      </c>
-      <c r="C98" t="inlineStr">
-        <is>
-          <t>{'64641'}</t>
-        </is>
-      </c>
-    </row>
-    <row r="99">
-      <c r="A99" t="n">
-        <v>131253</v>
-      </c>
-      <c r="B99" t="inlineStr">
-        <is>
-          <t>SENSOR_MAG_Y</t>
-        </is>
-      </c>
-      <c r="C99" t="inlineStr">
-        <is>
-          <t>{'1118'}</t>
-        </is>
-      </c>
-    </row>
-    <row r="100">
-      <c r="A100" t="n">
-        <v>131253</v>
-      </c>
-      <c r="B100" t="inlineStr">
-        <is>
-          <t>SENSOR_MAG_Z</t>
-        </is>
-      </c>
-      <c r="C100" t="inlineStr">
-        <is>
-          <t>{'64793'}</t>
-        </is>
-      </c>
-    </row>
-    <row r="101">
-      <c r="A101" t="n">
-        <v>131253</v>
-      </c>
-      <c r="B101" t="inlineStr">
-        <is>
-          <t>SENSOR_BARO</t>
-        </is>
-      </c>
-      <c r="C101" t="inlineStr">
-        <is>
-          <t>{'2088', '2977769'}</t>
-        </is>
-      </c>
-    </row>
-    <row r="102">
-      <c r="A102" t="n">
-        <v>131569</v>
-      </c>
-      <c r="B102" t="inlineStr">
-        <is>
-          <t>SENSOR_IMU_X</t>
-        </is>
-      </c>
-      <c r="C102" t="inlineStr">
-        <is>
-          <t>{'65063', '52'}</t>
-        </is>
-      </c>
-    </row>
-    <row r="103">
-      <c r="A103" t="n">
-        <v>131569</v>
-      </c>
-      <c r="B103" t="inlineStr">
-        <is>
-          <t>SENSOR_IMU_Y</t>
-        </is>
-      </c>
-      <c r="C103" t="inlineStr">
-        <is>
-          <t>{'104', '96'}</t>
-        </is>
-      </c>
-    </row>
-    <row r="104">
-      <c r="A104" t="n">
-        <v>131569</v>
-      </c>
-      <c r="B104" t="inlineStr">
-        <is>
-          <t>SENSOR_IMU_Z</t>
-        </is>
-      </c>
-      <c r="C104" t="inlineStr">
-        <is>
-          <t>{'2461', '63520'}</t>
-        </is>
-      </c>
-    </row>
-    <row r="105">
-      <c r="A105" t="n">
-        <v>131569</v>
-      </c>
-      <c r="B105" t="inlineStr">
-        <is>
-          <t>SENSOR_MAG_X</t>
-        </is>
-      </c>
-      <c r="C105" t="inlineStr">
-        <is>
-          <t>{'64425'}</t>
-        </is>
-      </c>
-    </row>
-    <row r="106">
-      <c r="A106" t="n">
-        <v>131569</v>
-      </c>
-      <c r="B106" t="inlineStr">
-        <is>
-          <t>SENSOR_MAG_Y</t>
-        </is>
-      </c>
-      <c r="C106" t="inlineStr">
-        <is>
-          <t>{'1136'}</t>
-        </is>
-      </c>
-    </row>
-    <row r="107">
-      <c r="A107" t="n">
-        <v>131569</v>
-      </c>
-      <c r="B107" t="inlineStr">
-        <is>
-          <t>SENSOR_MAG_Z</t>
-        </is>
-      </c>
-      <c r="C107" t="inlineStr">
-        <is>
-          <t>{'64790'}</t>
-        </is>
-      </c>
-    </row>
-    <row r="108">
-      <c r="A108" t="n">
-        <v>146457</v>
-      </c>
-      <c r="B108" t="inlineStr">
-        <is>
-          <t>SENSOR_IMU_X</t>
-        </is>
-      </c>
-      <c r="C108" t="inlineStr">
-        <is>
-          <t>{'65062', '65469'}</t>
-        </is>
-      </c>
-    </row>
-    <row r="109">
-      <c r="A109" t="n">
-        <v>146457</v>
-      </c>
-      <c r="B109" t="inlineStr">
-        <is>
-          <t>SENSOR_IMU_Y</t>
-        </is>
-      </c>
-      <c r="C109" t="inlineStr">
-        <is>
-          <t>{'118', '65304'}</t>
-        </is>
-      </c>
-    </row>
-    <row r="110">
-      <c r="A110" t="n">
-        <v>146457</v>
-      </c>
-      <c r="B110" t="inlineStr">
-        <is>
-          <t>SENSOR_IMU_Z</t>
-        </is>
-      </c>
-      <c r="C110" t="inlineStr">
-        <is>
-          <t>{'64204', '2241'}</t>
-        </is>
-      </c>
-    </row>
-    <row r="111">
-      <c r="A111" t="n">
-        <v>146457</v>
-      </c>
-      <c r="B111" t="inlineStr">
-        <is>
-          <t>SENSOR_MAG_X</t>
-        </is>
-      </c>
-      <c r="C111" t="inlineStr">
-        <is>
-          <t>{'64209'}</t>
-        </is>
-      </c>
-    </row>
-    <row r="112">
-      <c r="A112" t="n">
-        <v>146457</v>
-      </c>
-      <c r="B112" t="inlineStr">
-        <is>
-          <t>SENSOR_MAG_Y</t>
-        </is>
-      </c>
-      <c r="C112" t="inlineStr">
-        <is>
-          <t>{'918'}</t>
-        </is>
-      </c>
-    </row>
-    <row r="113">
-      <c r="A113" t="n">
-        <v>146457</v>
-      </c>
-      <c r="B113" t="inlineStr">
-        <is>
-          <t>SENSOR_MAG_Z</t>
-        </is>
-      </c>
-      <c r="C113" t="inlineStr">
-        <is>
-          <t>{'64761'}</t>
-        </is>
-      </c>
-    </row>
-    <row r="114">
-      <c r="A114" t="n">
-        <v>146457</v>
-      </c>
-      <c r="B114" t="inlineStr">
-        <is>
-          <t>SENSOR_BARO</t>
-        </is>
-      </c>
-      <c r="C114" t="inlineStr">
-        <is>
-          <t>{'3912278', '2174'}</t>
-        </is>
-      </c>
-    </row>
-    <row r="115">
-      <c r="A115" t="n">
-        <v>146563</v>
-      </c>
-      <c r="B115" t="inlineStr">
-        <is>
-          <t>SENSOR_IMU_X</t>
-        </is>
-      </c>
-      <c r="C115" t="inlineStr">
-        <is>
-          <t>{'446', '65401'}</t>
-        </is>
-      </c>
-    </row>
-    <row r="116">
-      <c r="A116" t="n">
+      <c r="A24" s="1" t="n">
         <v>146774</v>
       </c>
-      <c r="B116" t="inlineStr">
-        <is>
-          <t>SENSOR_IMU_X</t>
-        </is>
-      </c>
-      <c r="C116" t="inlineStr">
-        <is>
-          <t>{'54', '45'}</t>
-        </is>
-      </c>
-    </row>
-    <row r="117">
-      <c r="A117" t="n">
-        <v>146774</v>
-      </c>
-      <c r="B117" t="inlineStr">
-        <is>
-          <t>SENSOR_IMU_Y</t>
-        </is>
-      </c>
-      <c r="C117" t="inlineStr">
-        <is>
-          <t>{'48', '64657'}</t>
-        </is>
-      </c>
-    </row>
-    <row r="118">
-      <c r="A118" t="n">
-        <v>146774</v>
-      </c>
-      <c r="B118" t="inlineStr">
-        <is>
-          <t>SENSOR_IMU_Z</t>
-        </is>
-      </c>
-      <c r="C118" t="inlineStr">
-        <is>
-          <t>{'2550', '64365'}</t>
-        </is>
-      </c>
-    </row>
-    <row r="119">
-      <c r="A119" t="n">
-        <v>146774</v>
-      </c>
-      <c r="B119" t="inlineStr">
-        <is>
-          <t>SENSOR_MAG_X</t>
-        </is>
-      </c>
-      <c r="C119" t="inlineStr">
-        <is>
-          <t>{'64196'}</t>
-        </is>
-      </c>
-    </row>
-    <row r="120">
-      <c r="A120" t="n">
-        <v>146774</v>
-      </c>
-      <c r="B120" t="inlineStr">
-        <is>
-          <t>SENSOR_MAG_Y</t>
-        </is>
-      </c>
-      <c r="C120" t="inlineStr">
-        <is>
-          <t>{'789'}</t>
-        </is>
-      </c>
-    </row>
-    <row r="121">
-      <c r="A121" t="n">
-        <v>146774</v>
-      </c>
-      <c r="B121" t="inlineStr">
-        <is>
-          <t>SENSOR_MAG_Z</t>
-        </is>
-      </c>
-      <c r="C121" t="inlineStr">
-        <is>
-          <t>{'64752'}</t>
-        </is>
+      <c r="D24" t="n">
+        <v>45</v>
+      </c>
+      <c r="E24" t="n">
+        <v>54</v>
+      </c>
+      <c r="F24" t="n">
+        <v>48</v>
+      </c>
+      <c r="G24" t="n">
+        <v>64657</v>
+      </c>
+      <c r="H24" t="n">
+        <v>64365</v>
+      </c>
+      <c r="I24" t="n">
+        <v>2550</v>
+      </c>
+      <c r="J24" t="n">
+        <v>64196</v>
+      </c>
+      <c r="K24" t="n">
+        <v>789</v>
+      </c>
+      <c r="L24" t="n">
+        <v>64752</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="F1:G1"/>
+    <mergeCell ref="H1:I1"/>
+    <mergeCell ref="D1:E1"/>
+  </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>